<commit_message>
user id instead of user name identification (for AT)
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/users/Users-IUCT.xlsx
+++ b/Plancheck/plancheck_data/users/Users-IUCT.xlsx
@@ -138,9 +138,6 @@
     <t>brun</t>
   </si>
   <si>
-    <t>tournier</t>
-  </si>
-  <si>
     <t>parent</t>
   </si>
   <si>
@@ -472,6 +469,9 @@
   </si>
   <si>
     <t>Pasquier</t>
+  </si>
+  <si>
+    <t>barbier</t>
   </si>
 </sst>
 </file>
@@ -806,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,10 +883,10 @@
         <v>27</v>
       </c>
       <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" t="s">
         <v>59</v>
-      </c>
-      <c r="G3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -906,10 +906,10 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -929,10 +929,10 @@
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -952,10 +952,10 @@
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -975,10 +975,10 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -998,10 +998,10 @@
         <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1009,10 +1009,10 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
         <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>44</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
@@ -1021,10 +1021,10 @@
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1032,10 +1032,10 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
@@ -1044,10 +1044,10 @@
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1055,10 +1055,10 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
         <v>26</v>
@@ -1067,10 +1067,10 @@
         <v>28</v>
       </c>
       <c r="F11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" t="s">
         <v>117</v>
-      </c>
-      <c r="G11" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1078,10 +1078,10 @@
         <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
@@ -1090,10 +1090,10 @@
         <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1101,10 +1101,10 @@
         <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
@@ -1113,21 +1113,21 @@
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>150</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
@@ -1136,21 +1136,21 @@
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
@@ -1159,21 +1159,21 @@
         <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
@@ -1182,21 +1182,21 @@
         <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
         <v>26</v>
@@ -1205,22 +1205,22 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
         <v>78</v>
       </c>
-      <c r="C18" t="s">
-        <v>79</v>
-      </c>
       <c r="D18" t="s">
         <v>25</v>
       </c>
@@ -1228,21 +1228,21 @@
         <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
         <v>26</v>
@@ -1251,21 +1251,21 @@
         <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
@@ -1274,21 +1274,21 @@
         <v>29</v>
       </c>
       <c r="F20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
@@ -1297,21 +1297,21 @@
         <v>29</v>
       </c>
       <c r="F21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
@@ -1328,13 +1328,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1343,21 +1343,21 @@
         <v>29</v>
       </c>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1366,21 +1366,21 @@
         <v>29</v>
       </c>
       <c r="F24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
@@ -1389,21 +1389,21 @@
         <v>29</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
         <v>25</v>
@@ -1412,21 +1412,21 @@
         <v>29</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
         <v>26</v>
@@ -1435,21 +1435,21 @@
         <v>29</v>
       </c>
       <c r="F27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
         <v>25</v>
@@ -1458,21 +1458,21 @@
         <v>29</v>
       </c>
       <c r="F28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s">
         <v>25</v>
@@ -1481,21 +1481,21 @@
         <v>29</v>
       </c>
       <c r="F29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
         <v>25</v>
@@ -1504,21 +1504,21 @@
         <v>29</v>
       </c>
       <c r="F30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
         <v>25</v>
@@ -1527,21 +1527,21 @@
         <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
         <v>25</v>
@@ -1550,21 +1550,21 @@
         <v>29</v>
       </c>
       <c r="F32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D33" t="s">
         <v>25</v>
@@ -1573,21 +1573,21 @@
         <v>29</v>
       </c>
       <c r="F33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D34" t="s">
         <v>26</v>
@@ -1596,21 +1596,21 @@
         <v>29</v>
       </c>
       <c r="F34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" t="s">
         <v>59</v>
-      </c>
-      <c r="G34" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" t="s">
         <v>148</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>149</v>
-      </c>
-      <c r="C35" t="s">
-        <v>150</v>
       </c>
       <c r="D35" t="s">
         <v>26</v>
@@ -1619,10 +1619,10 @@
         <v>29</v>
       </c>
       <c r="F35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avant les tests de librairie
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/users/Users-IUCT.xlsx
+++ b/Plancheck/plancheck_data/users/Users-IUCT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="163">
   <si>
     <t>Id</t>
   </si>
@@ -499,6 +499,15 @@
   </si>
   <si>
     <t>Castex</t>
+  </si>
+  <si>
+    <t>zerbib</t>
+  </si>
+  <si>
+    <t>Caroline</t>
+  </si>
+  <si>
+    <t>Zerbib</t>
   </si>
 </sst>
 </file>
@@ -831,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:G38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,6 +1730,29 @@
         <v>59</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B39" t="s">
+        <v>161</v>
+      </c>
+      <c r="C39" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" t="s">
+        <v>118</v>
+      </c>
+      <c r="G39" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>